<commit_message>
Changes to run with nExpected cost = 0
</commit_message>
<xml_diff>
--- a/Result_15052025_v2.xlsx
+++ b/Result_15052025_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s194351_dtu_dk/Documents/Dokumenter/Master Thesis/MasterThesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="115_{B66BF699-D904-44A7-8AF5-DE1A3B4F1149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="115_{B66BF699-D904-44A7-8AF5-DE1A3B4F1149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65A58CB2-C107-454B-A4A1-E66435DC7D80}"/>
   <bookViews>
-    <workbookView xWindow="-14220" yWindow="-21600" windowWidth="43200" windowHeight="17085" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-16755" yWindow="-24135" windowWidth="57870" windowHeight="23550" activeTab="2" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Anticipation" sheetId="4" r:id="rId4"/>
     <sheet name="AnticipationNoALNS" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Comparison!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="1104">
   <si>
     <t>Method: BaseCase</t>
   </si>
@@ -3329,14 +3332,34 @@
   </si>
   <si>
     <t>13.5108</t>
+  </si>
+  <si>
+    <t>Time offline anticipation:</t>
+  </si>
+  <si>
+    <t>120 s</t>
+  </si>
+  <si>
+    <t>Time offline:</t>
+  </si>
+  <si>
+    <t>20 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3352,7 +3375,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3360,12 +3383,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3682,7 +3716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD95CD5A-99B3-4262-89F2-FCB1EE3A8753}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -3694,7 +3728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D2CF64-6329-4C31-96F3-2F859CEF5EA3}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5217,72 +5253,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D2CA70-E216-4585-939E-17849D61970C}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>353</v>
       </c>
@@ -5290,7 +5331,7 @@
         <v>354</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>-1.718</v>
@@ -5341,7 +5382,7 @@
         <v>3.0379999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>353</v>
       </c>
@@ -5349,7 +5390,7 @@
         <v>403</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>-3.28</v>
@@ -5400,7 +5441,7 @@
         <v>3.1048</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>353</v>
       </c>
@@ -5408,7 +5449,7 @@
         <v>354</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D4">
         <v>18.312000000000126</v>
@@ -5459,7 +5500,7 @@
         <v>-4.4238000000000017</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>353</v>
       </c>
@@ -5467,7 +5508,7 @@
         <v>403</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D5">
         <v>-7.6040000000000418</v>
@@ -5518,7 +5559,7 @@
         <v>-1.531600000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>353</v>
       </c>
@@ -5526,7 +5567,7 @@
         <v>354</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D6">
         <v>-4.4740000000001601</v>
@@ -5577,7 +5618,7 @@
         <v>-3.5295999999999967</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -5585,7 +5626,7 @@
         <v>403</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D7">
         <v>-3.7019999999997708</v>
@@ -5635,8 +5676,14 @@
       <c r="S7">
         <v>-4.039399999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="W7" t="s">
+        <v>1100</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>353</v>
       </c>
@@ -5644,7 +5691,7 @@
         <v>354</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D8">
         <v>-3.1700000000000728</v>
@@ -5694,8 +5741,14 @@
       <c r="S8">
         <v>-1.1945999999999994</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="W8" t="s">
+        <v>1102</v>
+      </c>
+      <c r="X8" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>353</v>
       </c>
@@ -5703,7 +5756,7 @@
         <v>403</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D9">
         <v>-9.204000000000633</v>
@@ -5754,66 +5807,66 @@
         <v>-3.8322000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>783</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-6.3319999999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-0.79200000000000004</v>
+      </c>
+      <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="D10">
-        <v>-6.3319999999999999</v>
-      </c>
-      <c r="E10">
-        <v>-0.79200000000000004</v>
-      </c>
-      <c r="F10">
+      <c r="G10" s="2">
+        <v>1.6000000000000005</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1588.9370078690754</v>
+      </c>
+      <c r="I10" s="2">
+        <v>-55.214849291131941</v>
+      </c>
+      <c r="J10" s="2">
+        <v>93</v>
+      </c>
+      <c r="K10" s="2">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>1.6000000000000005</v>
-      </c>
-      <c r="H10">
-        <v>1588.9370078690754</v>
-      </c>
-      <c r="I10">
-        <v>-55.214849291131941</v>
-      </c>
-      <c r="J10">
-        <v>93</v>
-      </c>
-      <c r="K10">
+      <c r="L10" s="2">
+        <v>-40.599999999999909</v>
+      </c>
+      <c r="M10" s="2">
+        <v>169.60000000000002</v>
+      </c>
+      <c r="N10" s="2">
+        <v>28.800000000000011</v>
+      </c>
+      <c r="O10" s="2">
         <v>0</v>
       </c>
-      <c r="L10">
-        <v>-40.599999999999909</v>
-      </c>
-      <c r="M10">
-        <v>169.60000000000002</v>
-      </c>
-      <c r="N10">
-        <v>28.800000000000011</v>
-      </c>
-      <c r="O10">
+      <c r="P10" s="2">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="Q10" s="2">
         <v>0</v>
       </c>
-      <c r="P10">
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
+      <c r="R10" s="2">
         <v>-3.4000000000000004</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="2">
         <v>2.7998000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>783</v>
       </c>
@@ -5821,7 +5874,7 @@
         <v>403</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>-6.3339999999999996</v>
@@ -5872,7 +5925,7 @@
         <v>1.5334000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>783</v>
       </c>
@@ -5880,7 +5933,7 @@
         <v>354</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D12">
         <v>-938.06200000000001</v>
@@ -5931,7 +5984,7 @@
         <v>-7.0793999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>783</v>
       </c>
@@ -5939,7 +5992,7 @@
         <v>403</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D13">
         <v>-938.05200000000002</v>
@@ -5990,7 +6043,7 @@
         <v>-7.5118000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>783</v>
       </c>
@@ -5998,7 +6051,7 @@
         <v>354</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D14">
         <v>-3600.6319999999996</v>
@@ -6049,7 +6102,7 @@
         <v>-2.0843999999999987</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>783</v>
       </c>
@@ -6057,7 +6110,7 @@
         <v>403</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D15">
         <v>-3600.6259999999997</v>
@@ -6108,7 +6161,7 @@
         <v>-1.3351999999999986</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>783</v>
       </c>
@@ -6116,7 +6169,7 @@
         <v>354</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D16">
         <v>-6010.558</v>
@@ -6175,7 +6228,7 @@
         <v>403</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D17">
         <v>-6010.482</v>
@@ -6227,6 +6280,31 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{F8D2CA70-E216-4585-939E-17849D61970C}"/>
+  <conditionalFormatting sqref="P2:P17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6235,7 +6313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CC564C-C923-457A-A033-3CAB2E06030C}">
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B46" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>